<commit_message>
reduce the call for features
ask only for key-values inthe pie index = tried but only made the app slower so I reverted it
</commit_message>
<xml_diff>
--- a/OSM features.xlsx
+++ b/OSM features.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3653" uniqueCount="1104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3653" uniqueCount="1105">
   <si>
     <t xml:space="preserve">subcategory</t>
   </si>
@@ -3325,6 +3325,9 @@
   </si>
   <si>
     <t xml:space="preserve">other landuse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">decorative greenery</t>
   </si>
   <si>
     <t xml:space="preserve">(to be) construction</t>
@@ -3443,8 +3446,8 @@
   </sheetPr>
   <dimension ref="A1:E859"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A202" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B263" activeCellId="0" sqref="B263"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C267" activeCellId="0" sqref="C267"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12268,8 +12271,8 @@
   </sheetPr>
   <dimension ref="A1:D221"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C40" activeCellId="0" sqref="C40"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A70" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B94" activeCellId="0" sqref="B94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13095,7 +13098,7 @@
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>568</v>
+        <v>1101</v>
       </c>
       <c r="B88" s="0" t="s">
         <v>493</v>
@@ -13123,7 +13126,7 @@
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>1101</v>
+        <v>1102</v>
       </c>
       <c r="B91" s="0" t="s">
         <v>493</v>
@@ -13137,7 +13140,7 @@
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>1101</v>
+        <v>1102</v>
       </c>
       <c r="B92" s="0" t="s">
         <v>493</v>
@@ -13151,7 +13154,7 @@
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>1101</v>
+        <v>1102</v>
       </c>
       <c r="B93" s="0" t="s">
         <v>493</v>
@@ -13165,7 +13168,7 @@
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B95" s="0" t="s">
         <v>640</v>
@@ -13179,7 +13182,7 @@
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B96" s="0" t="s">
         <v>640</v>
@@ -13193,7 +13196,7 @@
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B97" s="0" t="s">
         <v>640</v>
@@ -13207,7 +13210,7 @@
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B98" s="0" t="s">
         <v>640</v>
@@ -13221,7 +13224,7 @@
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B99" s="0" t="s">
         <v>640</v>
@@ -13235,7 +13238,7 @@
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B100" s="0" t="s">
         <v>640</v>
@@ -13277,7 +13280,7 @@
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B103" s="0" t="s">
         <v>640</v>
@@ -13305,12 +13308,12 @@
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B106" s="0" t="s">
         <v>640</v>
@@ -13324,7 +13327,7 @@
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B107" s="0" t="s">
         <v>640</v>
@@ -13338,7 +13341,7 @@
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B108" s="0" t="s">
         <v>640</v>
@@ -13352,7 +13355,7 @@
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B109" s="0" t="s">
         <v>640</v>
@@ -13366,7 +13369,7 @@
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B110" s="0" t="s">
         <v>640</v>
@@ -13380,7 +13383,7 @@
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B111" s="0" t="s">
         <v>640</v>
@@ -13394,7 +13397,7 @@
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B112" s="0" t="s">
         <v>640</v>
@@ -13408,7 +13411,7 @@
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B113" s="0" t="s">
         <v>640</v>
@@ -13422,7 +13425,7 @@
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B114" s="0" t="s">
         <v>640</v>
@@ -13436,7 +13439,7 @@
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B115" s="0" t="s">
         <v>640</v>
@@ -13450,7 +13453,7 @@
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B116" s="0" t="s">
         <v>640</v>
@@ -13464,7 +13467,7 @@
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B117" s="0" t="s">
         <v>640</v>
@@ -13478,7 +13481,7 @@
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B118" s="0" t="s">
         <v>640</v>
@@ -13492,7 +13495,7 @@
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B119" s="0" t="s">
         <v>640</v>
@@ -13506,7 +13509,7 @@
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B120" s="0" t="s">
         <v>640</v>
@@ -13520,7 +13523,7 @@
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B121" s="0" t="s">
         <v>640</v>
@@ -13534,7 +13537,7 @@
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B122" s="0" t="s">
         <v>640</v>
@@ -13548,7 +13551,7 @@
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B123" s="0" t="s">
         <v>640</v>
@@ -13562,7 +13565,7 @@
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B124" s="0" t="s">
         <v>640</v>
@@ -13576,12 +13579,12 @@
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B126" s="0" t="s">
         <v>640</v>
@@ -13595,7 +13598,7 @@
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B127" s="0" t="s">
         <v>640</v>
@@ -13609,7 +13612,7 @@
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B128" s="0" t="s">
         <v>640</v>
@@ -13623,7 +13626,7 @@
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B129" s="0" t="s">
         <v>640</v>
@@ -13637,7 +13640,7 @@
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B130" s="0" t="s">
         <v>640</v>
@@ -13651,7 +13654,7 @@
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B131" s="0" t="s">
         <v>640</v>
@@ -13665,7 +13668,7 @@
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B132" s="0" t="s">
         <v>640</v>
@@ -13679,7 +13682,7 @@
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B133" s="0" t="s">
         <v>640</v>
@@ -13693,7 +13696,7 @@
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B134" s="0" t="s">
         <v>640</v>
@@ -13707,7 +13710,7 @@
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B135" s="0" t="s">
         <v>640</v>
@@ -13721,7 +13724,7 @@
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B136" s="0" t="s">
         <v>640</v>
@@ -13735,7 +13738,7 @@
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B137" s="0" t="s">
         <v>640</v>
@@ -13749,7 +13752,7 @@
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B138" s="0" t="s">
         <v>640</v>
@@ -13763,7 +13766,7 @@
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B139" s="0" t="s">
         <v>640</v>
@@ -13777,7 +13780,7 @@
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B140" s="0" t="s">
         <v>640</v>
@@ -13791,7 +13794,7 @@
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B141" s="0" t="s">
         <v>640</v>
@@ -13805,7 +13808,7 @@
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B142" s="0" t="s">
         <v>640</v>
@@ -13819,7 +13822,7 @@
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B143" s="0" t="s">
         <v>640</v>
@@ -13833,7 +13836,7 @@
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B144" s="0" t="s">
         <v>640</v>
@@ -13847,7 +13850,7 @@
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B145" s="0" t="s">
         <v>640</v>
@@ -14652,7 +14655,7 @@
     </row>
     <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="0" t="s">
-        <v>1103</v>
+        <v>1104</v>
       </c>
       <c r="B218" s="0" t="s">
         <v>292</v>
@@ -14666,7 +14669,7 @@
     </row>
     <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="0" t="s">
-        <v>1103</v>
+        <v>1104</v>
       </c>
       <c r="B219" s="0" t="s">
         <v>292</v>
@@ -14680,7 +14683,7 @@
     </row>
     <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="0" t="s">
-        <v>1103</v>
+        <v>1104</v>
       </c>
       <c r="B220" s="0" t="s">
         <v>292</v>
@@ -14694,7 +14697,7 @@
     </row>
     <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="0" t="s">
-        <v>1103</v>
+        <v>1104</v>
       </c>
       <c r="B221" s="0" t="s">
         <v>292</v>
@@ -15325,7 +15328,7 @@
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>1101</v>
+        <v>1102</v>
       </c>
       <c r="B66" s="0" t="s">
         <v>493</v>
@@ -15339,7 +15342,7 @@
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>1101</v>
+        <v>1102</v>
       </c>
       <c r="B67" s="0" t="s">
         <v>493</v>
@@ -15353,7 +15356,7 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>1101</v>
+        <v>1102</v>
       </c>
       <c r="B68" s="0" t="s">
         <v>493</v>
@@ -15364,7 +15367,7 @@
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B70" s="0" t="s">
         <v>640</v>
@@ -15378,7 +15381,7 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B71" s="0" t="s">
         <v>640</v>
@@ -15392,7 +15395,7 @@
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B72" s="0" t="s">
         <v>640</v>
@@ -15406,7 +15409,7 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B73" s="0" t="s">
         <v>640</v>
@@ -15420,7 +15423,7 @@
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B74" s="0" t="s">
         <v>640</v>
@@ -15434,7 +15437,7 @@
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B75" s="0" t="s">
         <v>640</v>
@@ -15476,7 +15479,7 @@
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B78" s="0" t="s">
         <v>640</v>
@@ -15504,12 +15507,12 @@
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B81" s="0" t="s">
         <v>640</v>
@@ -15523,7 +15526,7 @@
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B82" s="0" t="s">
         <v>640</v>
@@ -15537,7 +15540,7 @@
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B83" s="0" t="s">
         <v>640</v>
@@ -15551,7 +15554,7 @@
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B84" s="0" t="s">
         <v>640</v>
@@ -15565,7 +15568,7 @@
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B85" s="0" t="s">
         <v>640</v>
@@ -15579,7 +15582,7 @@
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B86" s="0" t="s">
         <v>640</v>
@@ -15593,7 +15596,7 @@
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B87" s="0" t="s">
         <v>640</v>
@@ -15607,7 +15610,7 @@
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B88" s="0" t="s">
         <v>640</v>
@@ -15621,7 +15624,7 @@
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B89" s="0" t="s">
         <v>640</v>
@@ -15635,7 +15638,7 @@
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B90" s="0" t="s">
         <v>640</v>
@@ -15649,7 +15652,7 @@
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B91" s="0" t="s">
         <v>640</v>
@@ -15663,7 +15666,7 @@
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B92" s="0" t="s">
         <v>640</v>
@@ -15677,7 +15680,7 @@
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B93" s="0" t="s">
         <v>640</v>
@@ -15691,7 +15694,7 @@
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B94" s="0" t="s">
         <v>640</v>
@@ -15705,7 +15708,7 @@
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B95" s="0" t="s">
         <v>640</v>
@@ -15719,7 +15722,7 @@
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B96" s="0" t="s">
         <v>640</v>
@@ -15733,7 +15736,7 @@
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B97" s="0" t="s">
         <v>640</v>
@@ -15747,7 +15750,7 @@
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B98" s="0" t="s">
         <v>640</v>
@@ -15761,7 +15764,7 @@
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B99" s="0" t="s">
         <v>640</v>
@@ -15775,12 +15778,12 @@
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B101" s="0" t="s">
         <v>640</v>
@@ -15794,7 +15797,7 @@
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B102" s="0" t="s">
         <v>640</v>
@@ -15808,7 +15811,7 @@
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B103" s="0" t="s">
         <v>640</v>
@@ -15822,7 +15825,7 @@
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B104" s="0" t="s">
         <v>640</v>
@@ -15836,7 +15839,7 @@
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B105" s="0" t="s">
         <v>640</v>
@@ -15850,7 +15853,7 @@
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B106" s="0" t="s">
         <v>640</v>
@@ -15864,7 +15867,7 @@
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B107" s="0" t="s">
         <v>640</v>
@@ -15878,7 +15881,7 @@
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B108" s="0" t="s">
         <v>640</v>
@@ -15892,7 +15895,7 @@
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B109" s="0" t="s">
         <v>640</v>
@@ -15906,7 +15909,7 @@
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B110" s="0" t="s">
         <v>640</v>
@@ -15920,7 +15923,7 @@
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B111" s="0" t="s">
         <v>640</v>
@@ -15934,7 +15937,7 @@
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B112" s="0" t="s">
         <v>640</v>
@@ -15948,7 +15951,7 @@
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B113" s="0" t="s">
         <v>640</v>
@@ -15962,7 +15965,7 @@
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B114" s="0" t="s">
         <v>640</v>
@@ -15976,7 +15979,7 @@
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B115" s="0" t="s">
         <v>640</v>
@@ -15990,7 +15993,7 @@
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B116" s="0" t="s">
         <v>640</v>
@@ -16004,7 +16007,7 @@
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B117" s="0" t="s">
         <v>640</v>
@@ -16018,7 +16021,7 @@
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B118" s="0" t="s">
         <v>640</v>
@@ -16032,7 +16035,7 @@
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B119" s="0" t="s">
         <v>640</v>
@@ -16046,7 +16049,7 @@
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B120" s="0" t="s">
         <v>640</v>

</xml_diff>

<commit_message>
clean the pie chart
clean hover popup; do not include column names, add bold, clean value names, and add decimals to numbers
</commit_message>
<xml_diff>
--- a/OSM features.xlsx
+++ b/OSM features.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3653" uniqueCount="1105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3654" uniqueCount="1105">
   <si>
     <t xml:space="preserve">subcategory</t>
   </si>
@@ -3327,10 +3327,10 @@
     <t xml:space="preserve">other landuse</t>
   </si>
   <si>
-    <t xml:space="preserve">decorative greenery</t>
-  </si>
-  <si>
     <t xml:space="preserve">(to be) construction</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t xml:space="preserve">nature</t>
@@ -3446,8 +3446,8 @@
   </sheetPr>
   <dimension ref="A1:E859"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C267" activeCellId="0" sqref="C267"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A569" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P43" activeCellId="0" sqref="P43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12271,8 +12271,8 @@
   </sheetPr>
   <dimension ref="A1:D221"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A70" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B94" activeCellId="0" sqref="B94"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A72" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D94" activeCellId="0" sqref="D94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12770,7 +12770,7 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>1098</v>
+        <v>568</v>
       </c>
       <c r="B52" s="0" t="s">
         <v>493</v>
@@ -12841,7 +12841,7 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>1098</v>
+        <v>568</v>
       </c>
       <c r="B59" s="0" t="s">
         <v>493</v>
@@ -13098,7 +13098,7 @@
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>1101</v>
+        <v>568</v>
       </c>
       <c r="B88" s="0" t="s">
         <v>493</v>
@@ -13126,7 +13126,7 @@
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="B91" s="0" t="s">
         <v>493</v>
@@ -13140,7 +13140,7 @@
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="B92" s="0" t="s">
         <v>493</v>
@@ -13154,7 +13154,7 @@
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="B93" s="0" t="s">
         <v>493</v>
@@ -13164,6 +13164,11 @@
       </c>
       <c r="D93" s="0" t="s">
         <v>495</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B94" s="0" t="s">
+        <v>1102</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15328,7 +15333,7 @@
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="B66" s="0" t="s">
         <v>493</v>
@@ -15342,7 +15347,7 @@
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="B67" s="0" t="s">
         <v>493</v>
@@ -15356,7 +15361,7 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="B68" s="0" t="s">
         <v>493</v>

</xml_diff>